<commit_message>
Matouqin: update data input and plotting
</commit_message>
<xml_diff>
--- a/models/matouqin/Data/all_params.xlsx
+++ b/models/matouqin/Data/all_params.xlsx
@@ -456,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.23</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.29</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -640,7 +640,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
         <v>0.8</v>
@@ -655,7 +655,7 @@
         <v>0.0024</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0024</v>
+        <v>0.004</v>
       </c>
     </row>
   </sheetData>
@@ -740,10 +740,10 @@
         <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>0.005</v>
+        <v>0.0005</v>
       </c>
       <c r="G2" t="n">
         <v>19.97777777777777</v>
@@ -752,7 +752,7 @@
         <v>0.1295045749654566</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9065320247581963</v>
+        <v>0.009065320247581964</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +766,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -874,13 +874,13 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="J2" t="n">
-        <v>0.005</v>
+        <v>0.0005</v>
       </c>
       <c r="K2" t="n">
-        <v>1000</v>
+        <v>0.001</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -889,7 +889,53 @@
         <v>0.08024258719069129</v>
       </c>
       <c r="N2" t="n">
-        <v>0.4012129359534564</v>
+        <v>0.004012129359534564</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tank2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>500</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.08024258719069129</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.002407277615720738</v>
       </c>
     </row>
   </sheetData>
@@ -979,10 +1025,10 @@
         <v>0.7</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08</v>
+        <v>0.008</v>
       </c>
       <c r="F2" t="n">
-        <v>0.005</v>
+        <v>0.0005</v>
       </c>
       <c r="G2" t="n">
         <v>0.03954194444444445</v>
@@ -994,7 +1040,7 @@
         <v>0.08024258719069129</v>
       </c>
       <c r="J2" t="n">
-        <v>0.006419406975255303</v>
+        <v>0.0006419406975255303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>